<commit_message>
Updated FastFi to FastFiber
</commit_message>
<xml_diff>
--- a/projects/cymbal-kdb/src/raw_input/nlu-router-examples.xlsx
+++ b/projects/cymbal-kdb/src/raw_input/nlu-router-examples.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DYNAMIC_API" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,9 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{9DD840EB-C259-4F60-9C26-DF1214856B58}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{B714EF1E-518F-45DD-8EFE-7C9228C4E309}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{4C8D027A-1288-42D3-965A-6CD8C08AEE61}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{B714EF1E-518F-45DD-8EFE-7C9228C4E309}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{9DD840EB-C259-4F60-9C26-DF1214856B58}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2005,87 +2005,6 @@
     <t>Can you recommend a data plan for streaming</t>
   </si>
   <si>
-    <t>FastFi Broadband internet package recommendation for residential customer</t>
-  </si>
-  <si>
-    <t>How can I pay for FastFi service</t>
-  </si>
-  <si>
-    <t>Which FastFi Broadband internet package do you recommend for residential customers?</t>
-  </si>
-  <si>
-    <t>What is the recommended FastFi Broadband internet package for residential users?</t>
-  </si>
-  <si>
-    <t>Can you suggest a suitable FastFi Broadband internet package for residential customers?</t>
-  </si>
-  <si>
-    <t>How can I make payments for FastFi service?</t>
-  </si>
-  <si>
-    <t>What are the available payment methods for FastFi service?</t>
-  </si>
-  <si>
-    <t>Can you explain how I can pay for FastFi service?</t>
-  </si>
-  <si>
-    <t>What is Cymbal FastFi broadband internet ?</t>
-  </si>
-  <si>
-    <t>Where can I know more about Cymbal FastFi broadband internet ?</t>
-  </si>
-  <si>
-    <t>What are the advantages from Cymbal FastFi service?</t>
-  </si>
-  <si>
-    <t>How do you plan to expand Cymbal FastFi coverage?</t>
-  </si>
-  <si>
-    <t>How to subscribe Cymbal FastFi service ?</t>
-  </si>
-  <si>
-    <t>What is Cymbal FastFi broadband internet?</t>
-  </si>
-  <si>
-    <t>Can you explain what Cymbal FastFi broadband internet is?</t>
-  </si>
-  <si>
-    <t>I'm curious about Cymbal FastFi broadband internet.</t>
-  </si>
-  <si>
-    <t>Where can I find more information about Cymbal FastFi broadband internet?</t>
-  </si>
-  <si>
-    <t>Can you direct me to additional resources about Cymbal FastFi broadband internet?</t>
-  </si>
-  <si>
-    <t>Where can I access detailed information about Cymbal FastFi broadband internet?</t>
-  </si>
-  <si>
-    <t>What are the benefits of Cymbal FastFi service?</t>
-  </si>
-  <si>
-    <t>Can you outline the advantages of Cymbal FastFi service?</t>
-  </si>
-  <si>
-    <t>What benefits can I expect from Cymbal FastFi service?</t>
-  </si>
-  <si>
-    <t>What is your strategy for extending Cymbal FastFi coverage?</t>
-  </si>
-  <si>
-    <t>Can you provide insights into the expansion plans for Cymbal FastFi coverage?</t>
-  </si>
-  <si>
-    <t>How do I subscribe to Cymbal FastFi service?</t>
-  </si>
-  <si>
-    <t>What is the process for subscribing to Cymbal FastFi service?</t>
-  </si>
-  <si>
-    <t>Can you guide me on how to become a subscriber of Cymbal FastFi service?</t>
-  </si>
-  <si>
     <t>What is my balance for Calls to LifeApp Ooredoo and Tri</t>
   </si>
   <si>
@@ -2696,6 +2615,87 @@
   </si>
   <si>
     <t>Are there any entry limits for the BonusPlay game?</t>
+  </si>
+  <si>
+    <t>What is Cymbal FastFiber broadband internet ?</t>
+  </si>
+  <si>
+    <t>Where can I know more about Cymbal FastFiber broadband internet ?</t>
+  </si>
+  <si>
+    <t>What are the advantages from Cymbal FastFiber service?</t>
+  </si>
+  <si>
+    <t>How do you plan to expand Cymbal FastFiber coverage?</t>
+  </si>
+  <si>
+    <t>FastFiber Broadband internet package recommendation for residential customer</t>
+  </si>
+  <si>
+    <t>How can I pay for FastFiber service</t>
+  </si>
+  <si>
+    <t>How to subscribe Cymbal FastFiber service ?</t>
+  </si>
+  <si>
+    <t>What is Cymbal FastFiber broadband internet?</t>
+  </si>
+  <si>
+    <t>Can you explain what Cymbal FastFiber broadband internet is?</t>
+  </si>
+  <si>
+    <t>I'm curious about Cymbal FastFiber broadband internet.</t>
+  </si>
+  <si>
+    <t>Where can I find more information about Cymbal FastFiber broadband internet?</t>
+  </si>
+  <si>
+    <t>Can you direct me to additional resources about Cymbal FastFiber broadband internet?</t>
+  </si>
+  <si>
+    <t>Where can I access detailed information about Cymbal FastFiber broadband internet?</t>
+  </si>
+  <si>
+    <t>What are the benefits of Cymbal FastFiber service?</t>
+  </si>
+  <si>
+    <t>Can you outline the advantages of Cymbal FastFiber service?</t>
+  </si>
+  <si>
+    <t>What benefits can I expect from Cymbal FastFiber service?</t>
+  </si>
+  <si>
+    <t>What is your strategy for extending Cymbal FastFiber coverage?</t>
+  </si>
+  <si>
+    <t>Can you provide insights into the expansion plans for Cymbal FastFiber coverage?</t>
+  </si>
+  <si>
+    <t>Which FastFiber Broadband internet package do you recommend for residential customers?</t>
+  </si>
+  <si>
+    <t>What is the recommended FastFiber Broadband internet package for residential users?</t>
+  </si>
+  <si>
+    <t>Can you suggest a suitable FastFiber Broadband internet package for residential customers?</t>
+  </si>
+  <si>
+    <t>How can I make payments for FastFiber service?</t>
+  </si>
+  <si>
+    <t>What are the available payment methods for FastFiber service?</t>
+  </si>
+  <si>
+    <t>Can you explain how I can pay for FastFiber service?</t>
+  </si>
+  <si>
+    <t>How do I subscribe to Cymbal FastFiber service?</t>
+  </si>
+  <si>
+    <t>What is the process for subscribing to Cymbal FastFiber service?</t>
+  </si>
+  <si>
+    <t>Can you guide me on how to become a subscriber of Cymbal FastFiber service?</t>
   </si>
 </sst>
 </file>
@@ -2993,7 +2993,7 @@
   </sheetPr>
   <dimension ref="A1:Z277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+    <sheetView topLeftCell="A274" workbookViewId="0">
       <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
@@ -4094,7 +4094,7 @@
     </row>
     <row r="134" spans="1:2" ht="13" x14ac:dyDescent="0.6">
       <c r="A134" s="3" t="s">
-        <v>835</v>
+        <v>808</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>415</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="135" spans="1:2" ht="13" x14ac:dyDescent="0.6">
       <c r="A135" s="3" t="s">
-        <v>836</v>
+        <v>809</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>415</v>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="156" spans="1:2" ht="13" x14ac:dyDescent="0.6">
       <c r="A156" s="3" t="s">
-        <v>683</v>
+        <v>656</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>415</v>
@@ -5247,7 +5247,7 @@
   </sheetData>
   <autoFilter ref="A1:Z277"/>
   <customSheetViews>
-    <customSheetView guid="{B714EF1E-518F-45DD-8EFE-7C9228C4E309}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{9DD840EB-C259-4F60-9C26-DF1214856B58}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A1:AA538"/>
     </customSheetView>
@@ -5255,7 +5255,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A1:AA538"/>
     </customSheetView>
-    <customSheetView guid="{9DD840EB-C259-4F60-9C26-DF1214856B58}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{B714EF1E-518F-45DD-8EFE-7C9228C4E309}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A1:AA538"/>
     </customSheetView>
@@ -6879,7 +6879,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A201" t="s">
-        <v>857</v>
+        <v>830</v>
       </c>
       <c r="B201" t="s">
         <v>468</v>
@@ -6887,7 +6887,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A202" t="s">
-        <v>859</v>
+        <v>832</v>
       </c>
       <c r="B202" t="s">
         <v>468</v>
@@ -6895,7 +6895,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A203" t="s">
-        <v>860</v>
+        <v>833</v>
       </c>
       <c r="B203" t="s">
         <v>468</v>
@@ -6903,7 +6903,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A204" t="s">
-        <v>858</v>
+        <v>831</v>
       </c>
       <c r="B204" t="s">
         <v>468</v>
@@ -6911,7 +6911,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A205" t="s">
-        <v>861</v>
+        <v>834</v>
       </c>
       <c r="B205" t="s">
         <v>468</v>
@@ -6919,7 +6919,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A206" t="s">
-        <v>862</v>
+        <v>835</v>
       </c>
       <c r="B206" t="s">
         <v>468</v>
@@ -6937,8 +6937,8 @@
   </sheetPr>
   <dimension ref="A1:B406"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
@@ -6965,7 +6965,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A3" s="6" t="s">
-        <v>684</v>
+        <v>657</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>270</v>
@@ -6973,7 +6973,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A4" s="6" t="s">
-        <v>685</v>
+        <v>658</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>270</v>
@@ -6981,7 +6981,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A5" s="6" t="s">
-        <v>686</v>
+        <v>659</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>270</v>
@@ -6989,7 +6989,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A6" s="6" t="s">
-        <v>687</v>
+        <v>660</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>270</v>
@@ -7013,7 +7013,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A9" s="6" t="s">
-        <v>688</v>
+        <v>661</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>270</v>
@@ -7037,7 +7037,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A12" s="6" t="s">
-        <v>689</v>
+        <v>662</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>270</v>
@@ -7045,7 +7045,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A13" s="6" t="s">
-        <v>690</v>
+        <v>663</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>270</v>
@@ -7061,7 +7061,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A15" s="7" t="s">
-        <v>871</v>
+        <v>844</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>270</v>
@@ -7069,7 +7069,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A16" s="7" t="s">
-        <v>874</v>
+        <v>847</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>270</v>
@@ -7077,7 +7077,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A17" s="7" t="s">
-        <v>877</v>
+        <v>850</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>270</v>
@@ -7085,7 +7085,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A18" s="7" t="s">
-        <v>880</v>
+        <v>853</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>270</v>
@@ -7093,7 +7093,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A19" s="7" t="s">
-        <v>884</v>
+        <v>857</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>270</v>
@@ -7101,7 +7101,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A20" s="7" t="s">
-        <v>691</v>
+        <v>664</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>270</v>
@@ -7109,7 +7109,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A21" s="7" t="s">
-        <v>692</v>
+        <v>665</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>270</v>
@@ -7117,7 +7117,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A22" s="7" t="s">
-        <v>837</v>
+        <v>810</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>270</v>
@@ -7125,7 +7125,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A23" s="7" t="s">
-        <v>838</v>
+        <v>811</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>270</v>
@@ -7133,15 +7133,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A24" s="7" t="s">
-        <v>839</v>
+        <v>812</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:2" ht="26" x14ac:dyDescent="0.6">
       <c r="A25" s="7" t="s">
-        <v>840</v>
+        <v>813</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>270</v>
@@ -7149,7 +7149,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A26" s="7" t="s">
-        <v>693</v>
+        <v>666</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>270</v>
@@ -7157,7 +7157,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A27" s="7" t="s">
-        <v>694</v>
+        <v>667</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>270</v>
@@ -7165,7 +7165,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A28" s="7" t="s">
-        <v>695</v>
+        <v>668</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>270</v>
@@ -7181,7 +7181,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A30" s="7" t="s">
-        <v>696</v>
+        <v>669</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>270</v>
@@ -7189,7 +7189,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A31" s="7" t="s">
-        <v>697</v>
+        <v>670</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>270</v>
@@ -7205,7 +7205,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A33" s="7" t="s">
-        <v>698</v>
+        <v>671</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>270</v>
@@ -7213,7 +7213,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A34" s="7" t="s">
-        <v>699</v>
+        <v>672</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>270</v>
@@ -7221,7 +7221,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A35" s="7" t="s">
-        <v>700</v>
+        <v>673</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>270</v>
@@ -7229,7 +7229,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A36" s="7" t="s">
-        <v>701</v>
+        <v>674</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>270</v>
@@ -7237,7 +7237,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A37" s="7" t="s">
-        <v>702</v>
+        <v>675</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>270</v>
@@ -7245,7 +7245,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A38" s="7" t="s">
-        <v>703</v>
+        <v>676</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>270</v>
@@ -7253,7 +7253,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A39" s="7" t="s">
-        <v>704</v>
+        <v>677</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>270</v>
@@ -7269,7 +7269,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A41" s="7" t="s">
-        <v>705</v>
+        <v>678</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>270</v>
@@ -7293,7 +7293,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A44" s="7" t="s">
-        <v>706</v>
+        <v>679</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>270</v>
@@ -7301,7 +7301,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A45" s="7" t="s">
-        <v>707</v>
+        <v>680</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>270</v>
@@ -7309,7 +7309,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A46" s="7" t="s">
-        <v>708</v>
+        <v>681</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>270</v>
@@ -7317,7 +7317,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A47" s="7" t="s">
-        <v>709</v>
+        <v>682</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>270</v>
@@ -7325,7 +7325,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A48" s="7" t="s">
-        <v>710</v>
+        <v>683</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>270</v>
@@ -7333,7 +7333,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A49" s="7" t="s">
-        <v>711</v>
+        <v>684</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>270</v>
@@ -7341,7 +7341,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A50" s="7" t="s">
-        <v>712</v>
+        <v>685</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>270</v>
@@ -7349,7 +7349,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A51" s="7" t="s">
-        <v>713</v>
+        <v>686</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>270</v>
@@ -7357,7 +7357,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A52" s="7" t="s">
-        <v>714</v>
+        <v>687</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>270</v>
@@ -7365,7 +7365,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A53" s="7" t="s">
-        <v>867</v>
+        <v>840</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>270</v>
@@ -7373,7 +7373,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A54" s="7" t="s">
-        <v>715</v>
+        <v>688</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>270</v>
@@ -7381,7 +7381,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A55" s="7" t="s">
-        <v>716</v>
+        <v>689</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>270</v>
@@ -7389,7 +7389,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A56" s="7" t="s">
-        <v>717</v>
+        <v>690</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>270</v>
@@ -7397,7 +7397,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A57" s="7" t="s">
-        <v>863</v>
+        <v>836</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>270</v>
@@ -7437,7 +7437,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A62" s="7" t="s">
-        <v>853</v>
+        <v>826</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>270</v>
@@ -7461,7 +7461,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A65" t="s">
-        <v>664</v>
+        <v>860</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>270</v>
@@ -7469,7 +7469,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A66" t="s">
-        <v>665</v>
+        <v>861</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>270</v>
@@ -7477,7 +7477,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A67" t="s">
-        <v>666</v>
+        <v>862</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>270</v>
@@ -7485,7 +7485,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A68" t="s">
-        <v>667</v>
+        <v>863</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>270</v>
@@ -7493,7 +7493,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A69" t="s">
-        <v>656</v>
+        <v>864</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>270</v>
@@ -7501,7 +7501,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A70" t="s">
-        <v>657</v>
+        <v>865</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>270</v>
@@ -7509,7 +7509,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A71" t="s">
-        <v>668</v>
+        <v>866</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>270</v>
@@ -7573,7 +7573,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A79" t="s">
-        <v>718</v>
+        <v>691</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>270</v>
@@ -7621,7 +7621,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A85" t="s">
-        <v>719</v>
+        <v>692</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>270</v>
@@ -7653,7 +7653,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A89" t="s">
-        <v>720</v>
+        <v>693</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>270</v>
@@ -7669,7 +7669,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A91" t="s">
-        <v>721</v>
+        <v>694</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>270</v>
@@ -7717,7 +7717,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A97" t="s">
-        <v>722</v>
+        <v>695</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>270</v>
@@ -7725,7 +7725,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A98" t="s">
-        <v>723</v>
+        <v>696</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>270</v>
@@ -7733,7 +7733,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A99" t="s">
-        <v>724</v>
+        <v>697</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>270</v>
@@ -7741,7 +7741,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A100" t="s">
-        <v>725</v>
+        <v>698</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>270</v>
@@ -7749,7 +7749,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A101" t="s">
-        <v>726</v>
+        <v>699</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>270</v>
@@ -7757,7 +7757,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A102" t="s">
-        <v>727</v>
+        <v>700</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>270</v>
@@ -7765,7 +7765,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A103" t="s">
-        <v>728</v>
+        <v>701</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>270</v>
@@ -7773,7 +7773,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A104" t="s">
-        <v>729</v>
+        <v>702</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>270</v>
@@ -7781,7 +7781,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A105" t="s">
-        <v>730</v>
+        <v>703</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>270</v>
@@ -7789,7 +7789,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A106" t="s">
-        <v>731</v>
+        <v>704</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>270</v>
@@ -7797,7 +7797,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A107" t="s">
-        <v>732</v>
+        <v>705</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>270</v>
@@ -7805,7 +7805,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A108" t="s">
-        <v>733</v>
+        <v>706</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>270</v>
@@ -7861,7 +7861,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A115" t="s">
-        <v>734</v>
+        <v>707</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>270</v>
@@ -7869,7 +7869,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A116" t="s">
-        <v>735</v>
+        <v>708</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>270</v>
@@ -7877,7 +7877,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A117" t="s">
-        <v>736</v>
+        <v>709</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>270</v>
@@ -7885,7 +7885,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A118" t="s">
-        <v>737</v>
+        <v>710</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>270</v>
@@ -7893,7 +7893,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A119" t="s">
-        <v>738</v>
+        <v>711</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>270</v>
@@ -7901,7 +7901,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A120" t="s">
-        <v>739</v>
+        <v>712</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>270</v>
@@ -7933,7 +7933,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A124" t="s">
-        <v>740</v>
+        <v>713</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>270</v>
@@ -7941,7 +7941,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A125" t="s">
-        <v>741</v>
+        <v>714</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>270</v>
@@ -7949,7 +7949,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A126" t="s">
-        <v>742</v>
+        <v>715</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>270</v>
@@ -7957,7 +7957,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A127" t="s">
-        <v>690</v>
+        <v>663</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>270</v>
@@ -7965,7 +7965,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A128" t="s">
-        <v>743</v>
+        <v>716</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>270</v>
@@ -7973,7 +7973,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A129" t="s">
-        <v>744</v>
+        <v>717</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>270</v>
@@ -8005,7 +8005,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A133" t="s">
-        <v>871</v>
+        <v>844</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>270</v>
@@ -8013,7 +8013,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A134" t="s">
-        <v>872</v>
+        <v>845</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>270</v>
@@ -8021,7 +8021,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A135" t="s">
-        <v>873</v>
+        <v>846</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>270</v>
@@ -8029,7 +8029,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A136" t="s">
-        <v>874</v>
+        <v>847</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>270</v>
@@ -8037,7 +8037,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A137" t="s">
-        <v>875</v>
+        <v>848</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>270</v>
@@ -8045,7 +8045,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A138" t="s">
-        <v>876</v>
+        <v>849</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>270</v>
@@ -8053,7 +8053,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A139" t="s">
-        <v>877</v>
+        <v>850</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>270</v>
@@ -8061,7 +8061,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A140" t="s">
-        <v>878</v>
+        <v>851</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>270</v>
@@ -8069,7 +8069,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A141" t="s">
-        <v>879</v>
+        <v>852</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>270</v>
@@ -8077,7 +8077,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A142" t="s">
-        <v>881</v>
+        <v>854</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>270</v>
@@ -8085,7 +8085,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A143" t="s">
-        <v>882</v>
+        <v>855</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>270</v>
@@ -8093,7 +8093,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A144" t="s">
-        <v>883</v>
+        <v>856</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>270</v>
@@ -8101,7 +8101,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A145" t="s">
-        <v>884</v>
+        <v>857</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>270</v>
@@ -8109,7 +8109,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A146" t="s">
-        <v>885</v>
+        <v>858</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>270</v>
@@ -8117,7 +8117,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A147" t="s">
-        <v>886</v>
+        <v>859</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>270</v>
@@ -8125,7 +8125,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A148" t="s">
-        <v>691</v>
+        <v>664</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>270</v>
@@ -8133,7 +8133,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A149" t="s">
-        <v>745</v>
+        <v>718</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>270</v>
@@ -8141,7 +8141,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A150" t="s">
-        <v>746</v>
+        <v>719</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>270</v>
@@ -8149,7 +8149,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A151" t="s">
-        <v>747</v>
+        <v>720</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>270</v>
@@ -8157,7 +8157,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A152" t="s">
-        <v>748</v>
+        <v>721</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>270</v>
@@ -8165,7 +8165,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A153" t="s">
-        <v>749</v>
+        <v>722</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>270</v>
@@ -8173,7 +8173,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A154" t="s">
-        <v>841</v>
+        <v>814</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>270</v>
@@ -8181,7 +8181,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A155" t="s">
-        <v>842</v>
+        <v>815</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>270</v>
@@ -8189,7 +8189,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A156" t="s">
-        <v>843</v>
+        <v>816</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>270</v>
@@ -8197,7 +8197,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A157" t="s">
-        <v>844</v>
+        <v>817</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>270</v>
@@ -8205,7 +8205,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A158" t="s">
-        <v>845</v>
+        <v>818</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>270</v>
@@ -8213,7 +8213,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A159" t="s">
-        <v>846</v>
+        <v>819</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>270</v>
@@ -8221,7 +8221,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A160" t="s">
-        <v>847</v>
+        <v>820</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>270</v>
@@ -8229,7 +8229,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A161" t="s">
-        <v>848</v>
+        <v>821</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>270</v>
@@ -8237,7 +8237,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A162" t="s">
-        <v>849</v>
+        <v>822</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>270</v>
@@ -8245,7 +8245,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A163" t="s">
-        <v>850</v>
+        <v>823</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>270</v>
@@ -8253,7 +8253,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A164" t="s">
-        <v>851</v>
+        <v>824</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>270</v>
@@ -8261,7 +8261,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A165" t="s">
-        <v>852</v>
+        <v>825</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>270</v>
@@ -8269,7 +8269,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A166" t="s">
-        <v>750</v>
+        <v>723</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>270</v>
@@ -8277,7 +8277,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A167" t="s">
-        <v>751</v>
+        <v>724</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>270</v>
@@ -8285,7 +8285,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A168" t="s">
-        <v>752</v>
+        <v>725</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>270</v>
@@ -8293,7 +8293,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A169" t="s">
-        <v>753</v>
+        <v>726</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>270</v>
@@ -8301,7 +8301,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A170" t="s">
-        <v>754</v>
+        <v>727</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>270</v>
@@ -8309,7 +8309,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A171" t="s">
-        <v>755</v>
+        <v>728</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>270</v>
@@ -8317,7 +8317,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A172" t="s">
-        <v>756</v>
+        <v>729</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>270</v>
@@ -8325,7 +8325,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A173" t="s">
-        <v>757</v>
+        <v>730</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>270</v>
@@ -8333,7 +8333,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A174" t="s">
-        <v>758</v>
+        <v>731</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>270</v>
@@ -8365,7 +8365,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A178" t="s">
-        <v>759</v>
+        <v>732</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>270</v>
@@ -8373,7 +8373,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A179" t="s">
-        <v>760</v>
+        <v>733</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>270</v>
@@ -8381,7 +8381,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A180" t="s">
-        <v>761</v>
+        <v>734</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>270</v>
@@ -8389,7 +8389,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A181" t="s">
-        <v>762</v>
+        <v>735</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>270</v>
@@ -8397,7 +8397,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A182" t="s">
-        <v>763</v>
+        <v>736</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>270</v>
@@ -8405,7 +8405,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A183" t="s">
-        <v>764</v>
+        <v>737</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>270</v>
@@ -8437,7 +8437,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A187" t="s">
-        <v>765</v>
+        <v>738</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>270</v>
@@ -8445,7 +8445,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A188" t="s">
-        <v>766</v>
+        <v>739</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>270</v>
@@ -8453,7 +8453,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A189" t="s">
-        <v>767</v>
+        <v>740</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>270</v>
@@ -8461,7 +8461,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A190" t="s">
-        <v>768</v>
+        <v>741</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>270</v>
@@ -8469,7 +8469,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A191" t="s">
-        <v>769</v>
+        <v>742</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>270</v>
@@ -8477,7 +8477,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A192" t="s">
-        <v>770</v>
+        <v>743</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>270</v>
@@ -8485,7 +8485,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A193" t="s">
-        <v>771</v>
+        <v>744</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>270</v>
@@ -8493,7 +8493,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A194" t="s">
-        <v>772</v>
+        <v>745</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>270</v>
@@ -8501,7 +8501,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A195" t="s">
-        <v>773</v>
+        <v>746</v>
       </c>
       <c r="B195" s="3" t="s">
         <v>270</v>
@@ -8509,7 +8509,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A196" t="s">
-        <v>774</v>
+        <v>747</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>270</v>
@@ -8517,7 +8517,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A197" t="s">
-        <v>775</v>
+        <v>748</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>270</v>
@@ -8525,7 +8525,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A198" t="s">
-        <v>776</v>
+        <v>749</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>270</v>
@@ -8533,7 +8533,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A199" t="s">
-        <v>777</v>
+        <v>750</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>270</v>
@@ -8541,7 +8541,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A200" t="s">
-        <v>778</v>
+        <v>751</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>270</v>
@@ -8549,7 +8549,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A201" t="s">
-        <v>779</v>
+        <v>752</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>270</v>
@@ -8557,7 +8557,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A202" t="s">
-        <v>780</v>
+        <v>753</v>
       </c>
       <c r="B202" s="3" t="s">
         <v>270</v>
@@ -8565,7 +8565,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A203" t="s">
-        <v>781</v>
+        <v>754</v>
       </c>
       <c r="B203" s="3" t="s">
         <v>270</v>
@@ -8573,7 +8573,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A204" t="s">
-        <v>782</v>
+        <v>755</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>270</v>
@@ -8581,7 +8581,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A205" t="s">
-        <v>783</v>
+        <v>756</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>270</v>
@@ -8589,7 +8589,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A206" t="s">
-        <v>784</v>
+        <v>757</v>
       </c>
       <c r="B206" s="3" t="s">
         <v>270</v>
@@ -8597,7 +8597,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A207" t="s">
-        <v>785</v>
+        <v>758</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>270</v>
@@ -8629,7 +8629,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A211" t="s">
-        <v>786</v>
+        <v>759</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>270</v>
@@ -8637,7 +8637,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A212" t="s">
-        <v>787</v>
+        <v>760</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>270</v>
@@ -8645,7 +8645,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A213" t="s">
-        <v>788</v>
+        <v>761</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>270</v>
@@ -8701,7 +8701,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A220" t="s">
-        <v>789</v>
+        <v>762</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>270</v>
@@ -8709,7 +8709,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A221" t="s">
-        <v>790</v>
+        <v>763</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>270</v>
@@ -8717,7 +8717,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A222" t="s">
-        <v>791</v>
+        <v>764</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>270</v>
@@ -8725,7 +8725,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A223" t="s">
-        <v>792</v>
+        <v>765</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>270</v>
@@ -8733,7 +8733,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A224" t="s">
-        <v>793</v>
+        <v>766</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>270</v>
@@ -8741,7 +8741,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A225" t="s">
-        <v>794</v>
+        <v>767</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>270</v>
@@ -8749,7 +8749,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A226" t="s">
-        <v>795</v>
+        <v>768</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>270</v>
@@ -8757,7 +8757,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A227" t="s">
-        <v>796</v>
+        <v>769</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>270</v>
@@ -8765,7 +8765,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A228" t="s">
-        <v>797</v>
+        <v>770</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>270</v>
@@ -8773,7 +8773,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A229" t="s">
-        <v>798</v>
+        <v>771</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>270</v>
@@ -8781,7 +8781,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A230" t="s">
-        <v>799</v>
+        <v>772</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>270</v>
@@ -8789,7 +8789,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A231" t="s">
-        <v>800</v>
+        <v>773</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>270</v>
@@ -8797,7 +8797,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A232" t="s">
-        <v>801</v>
+        <v>774</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>270</v>
@@ -8805,7 +8805,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A233" t="s">
-        <v>802</v>
+        <v>775</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>270</v>
@@ -8813,7 +8813,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A234" t="s">
-        <v>803</v>
+        <v>776</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>270</v>
@@ -8821,7 +8821,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A235" t="s">
-        <v>804</v>
+        <v>777</v>
       </c>
       <c r="B235" s="3" t="s">
         <v>270</v>
@@ -8829,7 +8829,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A236" t="s">
-        <v>805</v>
+        <v>778</v>
       </c>
       <c r="B236" s="3" t="s">
         <v>270</v>
@@ -8837,7 +8837,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A237" t="s">
-        <v>806</v>
+        <v>779</v>
       </c>
       <c r="B237" s="3" t="s">
         <v>270</v>
@@ -8845,7 +8845,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A238" t="s">
-        <v>807</v>
+        <v>780</v>
       </c>
       <c r="B238" s="3" t="s">
         <v>270</v>
@@ -8853,7 +8853,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A239" t="s">
-        <v>808</v>
+        <v>781</v>
       </c>
       <c r="B239" s="3" t="s">
         <v>270</v>
@@ -8861,7 +8861,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A240" t="s">
-        <v>809</v>
+        <v>782</v>
       </c>
       <c r="B240" s="3" t="s">
         <v>270</v>
@@ -8869,7 +8869,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A241" t="s">
-        <v>810</v>
+        <v>783</v>
       </c>
       <c r="B241" s="3" t="s">
         <v>270</v>
@@ -8877,7 +8877,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A242" t="s">
-        <v>811</v>
+        <v>784</v>
       </c>
       <c r="B242" s="3" t="s">
         <v>270</v>
@@ -8885,7 +8885,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A243" t="s">
-        <v>812</v>
+        <v>785</v>
       </c>
       <c r="B243" s="3" t="s">
         <v>270</v>
@@ -8893,7 +8893,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A244" t="s">
-        <v>813</v>
+        <v>786</v>
       </c>
       <c r="B244" s="3" t="s">
         <v>270</v>
@@ -8901,7 +8901,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A245" t="s">
-        <v>814</v>
+        <v>787</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>270</v>
@@ -8909,7 +8909,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A246" t="s">
-        <v>815</v>
+        <v>788</v>
       </c>
       <c r="B246" s="3" t="s">
         <v>270</v>
@@ -8917,7 +8917,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A247" t="s">
-        <v>868</v>
+        <v>841</v>
       </c>
       <c r="B247" s="3" t="s">
         <v>270</v>
@@ -8925,7 +8925,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A248" t="s">
-        <v>869</v>
+        <v>842</v>
       </c>
       <c r="B248" s="3" t="s">
         <v>270</v>
@@ -8933,7 +8933,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A249" t="s">
-        <v>870</v>
+        <v>843</v>
       </c>
       <c r="B249" s="3" t="s">
         <v>270</v>
@@ -8941,7 +8941,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A250" t="s">
-        <v>816</v>
+        <v>789</v>
       </c>
       <c r="B250" s="3" t="s">
         <v>270</v>
@@ -8949,7 +8949,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A251" t="s">
-        <v>817</v>
+        <v>790</v>
       </c>
       <c r="B251" s="3" t="s">
         <v>270</v>
@@ -8957,7 +8957,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A252" t="s">
-        <v>818</v>
+        <v>791</v>
       </c>
       <c r="B252" s="3" t="s">
         <v>270</v>
@@ -8965,7 +8965,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A253" t="s">
-        <v>819</v>
+        <v>792</v>
       </c>
       <c r="B253" s="3" t="s">
         <v>270</v>
@@ -8973,7 +8973,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A254" t="s">
-        <v>820</v>
+        <v>793</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>270</v>
@@ -8981,7 +8981,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A255" t="s">
-        <v>821</v>
+        <v>794</v>
       </c>
       <c r="B255" s="3" t="s">
         <v>270</v>
@@ -8989,7 +8989,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A256" t="s">
-        <v>717</v>
+        <v>690</v>
       </c>
       <c r="B256" s="3" t="s">
         <v>270</v>
@@ -8997,7 +8997,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A257" t="s">
-        <v>822</v>
+        <v>795</v>
       </c>
       <c r="B257" s="3" t="s">
         <v>270</v>
@@ -9005,7 +9005,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A258" t="s">
-        <v>823</v>
+        <v>796</v>
       </c>
       <c r="B258" s="3" t="s">
         <v>270</v>
@@ -9013,7 +9013,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A259" t="s">
-        <v>864</v>
+        <v>837</v>
       </c>
       <c r="B259" s="3" t="s">
         <v>270</v>
@@ -9021,7 +9021,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A260" t="s">
-        <v>865</v>
+        <v>838</v>
       </c>
       <c r="B260" s="3" t="s">
         <v>270</v>
@@ -9029,7 +9029,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A261" t="s">
-        <v>866</v>
+        <v>839</v>
       </c>
       <c r="B261" s="3" t="s">
         <v>270</v>
@@ -9133,7 +9133,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A274" t="s">
-        <v>854</v>
+        <v>827</v>
       </c>
       <c r="B274" s="3" t="s">
         <v>270</v>
@@ -9141,7 +9141,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A275" t="s">
-        <v>855</v>
+        <v>828</v>
       </c>
       <c r="B275" s="3" t="s">
         <v>270</v>
@@ -9149,7 +9149,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A276" t="s">
-        <v>856</v>
+        <v>829</v>
       </c>
       <c r="B276" s="3" t="s">
         <v>270</v>
@@ -9205,7 +9205,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A283" t="s">
-        <v>669</v>
+        <v>867</v>
       </c>
       <c r="B283" s="3" t="s">
         <v>270</v>
@@ -9213,7 +9213,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A284" t="s">
-        <v>670</v>
+        <v>868</v>
       </c>
       <c r="B284" s="3" t="s">
         <v>270</v>
@@ -9221,7 +9221,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A285" t="s">
-        <v>671</v>
+        <v>869</v>
       </c>
       <c r="B285" s="3" t="s">
         <v>270</v>
@@ -9229,7 +9229,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A286" t="s">
-        <v>672</v>
+        <v>870</v>
       </c>
       <c r="B286" s="3" t="s">
         <v>270</v>
@@ -9237,7 +9237,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A287" t="s">
-        <v>673</v>
+        <v>871</v>
       </c>
       <c r="B287" s="3" t="s">
         <v>270</v>
@@ -9245,7 +9245,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A288" t="s">
-        <v>674</v>
+        <v>872</v>
       </c>
       <c r="B288" s="3" t="s">
         <v>270</v>
@@ -9253,7 +9253,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A289" t="s">
-        <v>675</v>
+        <v>873</v>
       </c>
       <c r="B289" s="3" t="s">
         <v>270</v>
@@ -9261,7 +9261,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A290" t="s">
-        <v>676</v>
+        <v>874</v>
       </c>
       <c r="B290" s="3" t="s">
         <v>270</v>
@@ -9269,7 +9269,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A291" t="s">
-        <v>677</v>
+        <v>875</v>
       </c>
       <c r="B291" s="3" t="s">
         <v>270</v>
@@ -9277,7 +9277,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A292" t="s">
-        <v>667</v>
+        <v>863</v>
       </c>
       <c r="B292" s="3" t="s">
         <v>270</v>
@@ -9285,7 +9285,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A293" t="s">
-        <v>678</v>
+        <v>876</v>
       </c>
       <c r="B293" s="3" t="s">
         <v>270</v>
@@ -9293,7 +9293,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A294" t="s">
-        <v>679</v>
+        <v>877</v>
       </c>
       <c r="B294" s="3" t="s">
         <v>270</v>
@@ -9301,7 +9301,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A295" t="s">
-        <v>658</v>
+        <v>878</v>
       </c>
       <c r="B295" s="3" t="s">
         <v>270</v>
@@ -9309,7 +9309,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A296" t="s">
-        <v>659</v>
+        <v>879</v>
       </c>
       <c r="B296" s="3" t="s">
         <v>270</v>
@@ -9317,7 +9317,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A297" t="s">
-        <v>660</v>
+        <v>880</v>
       </c>
       <c r="B297" s="3" t="s">
         <v>270</v>
@@ -9325,7 +9325,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A298" t="s">
-        <v>661</v>
+        <v>881</v>
       </c>
       <c r="B298" s="3" t="s">
         <v>270</v>
@@ -9333,7 +9333,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A299" t="s">
-        <v>662</v>
+        <v>882</v>
       </c>
       <c r="B299" s="3" t="s">
         <v>270</v>
@@ -9341,7 +9341,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A300" t="s">
-        <v>663</v>
+        <v>883</v>
       </c>
       <c r="B300" s="3" t="s">
         <v>270</v>
@@ -9349,7 +9349,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A301" t="s">
-        <v>680</v>
+        <v>884</v>
       </c>
       <c r="B301" s="3" t="s">
         <v>270</v>
@@ -9357,7 +9357,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A302" t="s">
-        <v>681</v>
+        <v>885</v>
       </c>
       <c r="B302" s="3" t="s">
         <v>270</v>
@@ -9365,7 +9365,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A303" t="s">
-        <v>682</v>
+        <v>886</v>
       </c>
       <c r="B303" s="3" t="s">
         <v>270</v>
@@ -9517,7 +9517,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A322" t="s">
-        <v>718</v>
+        <v>691</v>
       </c>
       <c r="B322" s="3" t="s">
         <v>270</v>
@@ -9525,7 +9525,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A323" t="s">
-        <v>824</v>
+        <v>797</v>
       </c>
       <c r="B323" s="3" t="s">
         <v>270</v>
@@ -9533,7 +9533,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A324" t="s">
-        <v>825</v>
+        <v>798</v>
       </c>
       <c r="B324" s="3" t="s">
         <v>270</v>
@@ -9661,7 +9661,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A340" t="s">
-        <v>826</v>
+        <v>799</v>
       </c>
       <c r="B340" s="3" t="s">
         <v>270</v>
@@ -9669,7 +9669,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A341" t="s">
-        <v>827</v>
+        <v>800</v>
       </c>
       <c r="B341" s="3" t="s">
         <v>270</v>
@@ -9677,7 +9677,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A342" t="s">
-        <v>828</v>
+        <v>801</v>
       </c>
       <c r="B342" s="3" t="s">
         <v>270</v>
@@ -9757,7 +9757,7 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A352" t="s">
-        <v>829</v>
+        <v>802</v>
       </c>
       <c r="B352" s="3" t="s">
         <v>270</v>
@@ -9765,7 +9765,7 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A353" t="s">
-        <v>830</v>
+        <v>803</v>
       </c>
       <c r="B353" s="3" t="s">
         <v>270</v>
@@ -9773,7 +9773,7 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A354" t="s">
-        <v>831</v>
+        <v>804</v>
       </c>
       <c r="B354" s="3" t="s">
         <v>270</v>
@@ -9797,7 +9797,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A357" t="s">
-        <v>832</v>
+        <v>805</v>
       </c>
       <c r="B357" s="3" t="s">
         <v>270</v>
@@ -9805,7 +9805,7 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A358" t="s">
-        <v>721</v>
+        <v>694</v>
       </c>
       <c r="B358" s="3" t="s">
         <v>270</v>
@@ -9813,7 +9813,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A359" t="s">
-        <v>833</v>
+        <v>806</v>
       </c>
       <c r="B359" s="3" t="s">
         <v>270</v>
@@ -9821,7 +9821,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A360" t="s">
-        <v>834</v>
+        <v>807</v>
       </c>
       <c r="B360" s="3" t="s">
         <v>270</v>

</xml_diff>